<commit_message>
#NITN *.xlsx results, test images
</commit_message>
<xml_diff>
--- a/Results/ResultsTest.xlsx
+++ b/Results/ResultsTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nasta\OneDrive\Desktop\Licenta-repo\Licenta\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBAC492F-B792-48B6-8AD1-8DE4C182922C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2EA11F-A0E4-4160-A921-6F4AC943BF7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8240" yWindow="1330" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Index</t>
   </si>
@@ -85,36 +85,12 @@
     <t>Carsc.png</t>
   </si>
   <si>
-    <t>TEST1.jpg</t>
-  </si>
-  <si>
-    <t>TEST2.jpg</t>
-  </si>
-  <si>
-    <t>TEST3.jpg</t>
-  </si>
-  <si>
     <t>TEST4.jpg</t>
   </si>
   <si>
-    <t>TEST5.jpg</t>
-  </si>
-  <si>
-    <t>TEST6.jpg</t>
-  </si>
-  <si>
-    <t>TEST7.jpg</t>
-  </si>
-  <si>
-    <t>TEST8.jpg</t>
-  </si>
-  <si>
     <t>TEST9.jpg</t>
   </si>
   <si>
-    <t>TEST10.jpg</t>
-  </si>
-  <si>
     <t>TEST11.jpg</t>
   </si>
   <si>
@@ -169,16 +145,7 @@
     <t>TEST28.jpg</t>
   </si>
   <si>
-    <t>TEST.jpg</t>
-  </si>
-  <si>
     <t>Nivel detectie</t>
-  </si>
-  <si>
-    <t>Dificultate detectie</t>
-  </si>
-  <si>
-    <t>Scor</t>
   </si>
 </sst>
 </file>
@@ -514,20 +481,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E152"/>
+  <dimension ref="A1:C143"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="8.7265625" style="2"/>
+    <col min="2" max="2" width="17.08984375" style="2" customWidth="1"/>
     <col min="3" max="3" width="19.26953125" style="2" customWidth="1"/>
     <col min="4" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -535,16 +503,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
@@ -552,7 +517,10 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
@@ -560,7 +528,10 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -568,7 +539,10 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
@@ -576,7 +550,10 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
@@ -584,7 +561,10 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
@@ -592,7 +572,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
       <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
@@ -600,7 +583,10 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
       <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
@@ -608,7 +594,10 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
       <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
@@ -616,7 +605,10 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
@@ -624,7 +616,10 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
@@ -632,7 +627,10 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
       <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
@@ -640,7 +638,10 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
       <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
@@ -648,7 +649,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
       <c r="B15" s="2" t="s">
         <v>15</v>
       </c>
@@ -656,251 +660,266 @@
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
       <c r="B16" s="2" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="C16" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
       <c r="B17" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C17" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B18" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="C18" s="1">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="1">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="1">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="1">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="1">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B20" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="1">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="1">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B23" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="1">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B24" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="1">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
       <c r="B25" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C25" s="1">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
       <c r="B26" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C26" s="1">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
       <c r="B27" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C27" s="1">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
       <c r="B28" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C28" s="1">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
       <c r="B29" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C29" s="1">
         <v>82</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
       <c r="B30" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C30" s="1">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="2">
+        <v>30</v>
+      </c>
       <c r="B31" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C31" s="1">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="2">
+        <v>31</v>
+      </c>
       <c r="B32" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C32" s="1">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" s="2">
+        <v>32</v>
+      </c>
       <c r="B33" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C33" s="1">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" s="2">
+        <v>33</v>
+      </c>
       <c r="B34" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C34" s="1">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="2">
+        <v>34</v>
+      </c>
       <c r="B35" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C35" s="1">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B36" s="2" t="s">
-        <v>35</v>
-      </c>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C36" s="1">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B37" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C37" s="1">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B38" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C38" s="1">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B39" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C39" s="1">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B40" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C40" s="1">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B41" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C41" s="1">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B42" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C42" s="1">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B43" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C43" s="1">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B44" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C44" s="1">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C45" s="1">
-        <f>AVERAGE(C2:C44)</f>
-        <v>59.697674418604649</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.35">
+        <f>AVERAGE(C2:C35)</f>
+        <v>68.17647058823529</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C37" s="1"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C39" s="1"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C40" s="1"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C41" s="1"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C42" s="1"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C43" s="1"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C44" s="1"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C45" s="1"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C48" s="1"/>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.35">
@@ -1187,33 +1206,6 @@
     </row>
     <row r="143" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C143" s="1"/>
-    </row>
-    <row r="144" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C144" s="1"/>
-    </row>
-    <row r="145" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C145" s="1"/>
-    </row>
-    <row r="146" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C146" s="1"/>
-    </row>
-    <row r="147" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C147" s="1"/>
-    </row>
-    <row r="148" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C148" s="1"/>
-    </row>
-    <row r="149" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C149" s="1"/>
-    </row>
-    <row r="150" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C150" s="1"/>
-    </row>
-    <row r="151" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C151" s="1"/>
-    </row>
-    <row r="152" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C152" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>